<commit_message>
updated script 02 for eDNA bioinfo
</commit_message>
<xml_diff>
--- a/eDNA/example_output/ASV_breakdown.xlsx
+++ b/eDNA/example_output/ASV_breakdown.xlsx
@@ -1876,17 +1876,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5e733a21f67e541f28ed4bf4fe025044</t>
+          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Paralichthys dentatus</t>
+          <t>Centropristis striata</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Summer flounder</t>
+          <t>Black sea bass</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1904,17 +1904,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
+          <t>5e733a21f67e541f28ed4bf4fe025044</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Centropristis striata</t>
+          <t>Paralichthys dentatus</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Black sea bass</t>
+          <t>Summer flounder</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">

</xml_diff>